<commit_message>
Agrego datos en planilla
</commit_message>
<xml_diff>
--- a/DisenioEstructurasGarridoNeyraVera.xlsx
+++ b/DisenioEstructurasGarridoNeyraVera.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Apellido</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>https://github.com/GarGiN81/tateti.git</t>
+  </si>
+  <si>
+    <t>gustavo.neyra@est.fi.uncoma.edu.ar</t>
+  </si>
+  <si>
+    <t>FAI-2020</t>
+  </si>
+  <si>
+    <t>GENEY11</t>
+  </si>
+  <si>
+    <t>FAI-3602</t>
+  </si>
+  <si>
+    <t>guillermo.vera@est.fi.uncoma.edu.ar</t>
+  </si>
+  <si>
+    <t>guilleV12</t>
   </si>
 </sst>
 </file>
@@ -187,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,6 +221,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -487,7 +506,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,30 +566,46 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G4" s="8"/>
     </row>
   </sheetData>
@@ -580,8 +615,10 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3" display="mailto:gustavo.neyra@est.fi.uncoma.edu.ar"/>
+    <hyperlink ref="D4" r:id="rId4" display="mailto:guillermo.vera@est.fi.uncoma.edu.ar"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>